<commit_message>
Add Contest1ParallelPerformanceData.xlsx and RayleighTaylorPerformanceData.xlsx
</commit_message>
<xml_diff>
--- a/sheet05/data/RayleighTaylorPerformanceData.xlsx
+++ b/sheet05/data/RayleighTaylorPerformanceData.xlsx
@@ -5,20 +5,34 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\tobias\performance_data_2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\manuel\TUM\MolSim-WS23-24\sheet05\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56EC26AC-FE64-4BD9-A3BB-71A9A34880FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87E25CE2-0A98-4314-8BFD-A6C3A5FF7400}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="10650" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -172,16 +186,13 @@
               <a:buFontTx/>
               <a:buNone/>
               <a:tabLst/>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr>
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:sysClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
@@ -1016,11 +1027,707 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="339467295"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-DE" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Contest1 / Rayleigh-Taylor-Instability 2D (10,000 Particles)</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-DE" sz="1200"/>
+              <a:t>Simulation</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="de-DE" sz="1200" baseline="0"/>
+              <a:t> of 1000 Iterations on CoolMUC</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Speedup (cluster:serial)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Tabelle1!$B$5:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>96</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$H$5:$H$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.1976214233704592</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.1284697021567953</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.939894741321833</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.5110713209353452</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.5729190943152691</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-6EBB-4A00-9535-6ED07928F3D1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Speedup (cluster:inter)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Tabelle1!$B$5:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>96</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$J$5:$J$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-6EBB-4A00-9535-6ED07928F3D1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="104290431"/>
+        <c:axId val="296003935"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="104290431"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>#Threads</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="296003935"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="296003935"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>Speedup</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="104290431"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1144,6 +1851,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1660,20 +2407,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>395286</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>138111</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>378957</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>21090</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>152399</xdr:colOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>133349</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>28574</xdr:rowOff>
+      <xdr:rowOff>96610</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1698,7 +2961,152 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>351064</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>102735</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>104095</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Diagramm 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0655FD03-EE9B-450F-9241-E027245CBA6D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Tabelle1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="5">
+          <cell r="B5">
+            <v>1</v>
+          </cell>
+          <cell r="H5">
+            <v>1</v>
+          </cell>
+          <cell r="I5">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="B6">
+            <v>2</v>
+          </cell>
+          <cell r="H6">
+            <v>1.1570277529095792</v>
+          </cell>
+          <cell r="I6">
+            <v>1.2215770171149145</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="B7">
+            <v>4</v>
+          </cell>
+          <cell r="H7">
+            <v>1.6987381703470033</v>
+          </cell>
+          <cell r="I7">
+            <v>1.854756380510441</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="B8">
+            <v>8</v>
+          </cell>
+          <cell r="H8">
+            <v>2.2673684210526313</v>
+          </cell>
+          <cell r="I8">
+            <v>2.3415348564733449</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="B9">
+            <v>16</v>
+          </cell>
+          <cell r="H9">
+            <v>1.619548872180451</v>
+          </cell>
+          <cell r="I9">
+            <v>2.6452680344142951</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="B10">
+            <v>28</v>
+          </cell>
+          <cell r="H10">
+            <v>0.39206406989443027</v>
+          </cell>
+          <cell r="I10">
+            <v>2.8570407433881342</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="B11">
+            <v>56</v>
+          </cell>
+          <cell r="I11">
+            <v>1.8686302010285181</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="B12">
+            <v>72</v>
+          </cell>
+          <cell r="I12">
+            <v>1.4749077490774907</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="B13">
+            <v>96</v>
+          </cell>
+          <cell r="I13">
+            <v>0.66649991662497921</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1964,24 +3372,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:F13"/>
+  <dimension ref="B2:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R19" sqref="R19"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12.3046875" customWidth="1"/>
+    <col min="3" max="3" width="13.3046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.4">
       <c r="C3" t="s">
         <v>4</v>
       </c>
@@ -1989,7 +3397,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B4" t="s">
         <v>1</v>
       </c>
@@ -2006,7 +3414,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B5">
         <v>1</v>
       </c>
@@ -2016,8 +3424,16 @@
       <c r="D5">
         <v>160842.557654</v>
       </c>
+      <c r="H5">
+        <f>$C$5/C5</f>
+        <v>1</v>
+      </c>
+      <c r="J5" t="e">
+        <f>$E$5/E5</f>
+        <v>#DIV/0!</v>
+      </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B6">
         <v>2</v>
       </c>
@@ -2027,8 +3443,16 @@
       <c r="D6">
         <v>192628.49283599999</v>
       </c>
+      <c r="H6">
+        <f t="shared" ref="H6:H13" si="0">$C$5/C6</f>
+        <v>1.1976214233704592</v>
+      </c>
+      <c r="J6" t="e">
+        <f t="shared" ref="J6:J13" si="1">$E$5/E6</f>
+        <v>#DIV/0!</v>
+      </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B7">
         <v>4</v>
       </c>
@@ -2038,8 +3462,16 @@
       <c r="D7">
         <v>342454.025547</v>
       </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>2.1284697021567953</v>
+      </c>
+      <c r="J7" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B8">
         <v>8</v>
       </c>
@@ -2049,8 +3481,16 @@
       <c r="D8">
         <v>472860.18942800001</v>
       </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>2.939894741321833</v>
+      </c>
+      <c r="J8" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B9">
         <v>16</v>
       </c>
@@ -2060,8 +3500,16 @@
       <c r="D9">
         <v>886414.80667299998</v>
       </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>5.5110713209353452</v>
+      </c>
+      <c r="J9" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B10">
         <v>28</v>
       </c>
@@ -2077,8 +3525,16 @@
       <c r="F10">
         <v>1580353.0508719999</v>
       </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>5.5729190943152691</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B11">
         <v>56</v>
       </c>
@@ -2088,8 +3544,16 @@
       <c r="F11">
         <v>1822091.0316679999</v>
       </c>
+      <c r="H11" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B12">
         <v>72</v>
       </c>
@@ -2099,8 +3563,16 @@
       <c r="F12">
         <v>1536948.2355829999</v>
       </c>
+      <c r="H12" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B13">
         <v>96</v>
       </c>
@@ -2109,6 +3581,14 @@
       </c>
       <c r="F13">
         <v>1076472.614537</v>
+      </c>
+      <c r="H13" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed deprecated data, and generated new plots
</commit_message>
<xml_diff>
--- a/sheet05/data/RayleighTaylorPerformanceData.xlsx
+++ b/sheet05/data/RayleighTaylorPerformanceData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\tobias\MolSim-WS23-24\sheet05\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\tobias\MolSimPresentation\sheet05\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C08A6306-9F19-406E-A69A-2789EC76629C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2B9B3C6-8612-406C-833A-47841A5204A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -303,7 +303,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -325,6 +325,12 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -343,13 +349,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -12678,7 +12677,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:N77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B64" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="K77" sqref="K77"/>
     </sheetView>
   </sheetViews>
@@ -12901,44 +12900,44 @@
     </row>
     <row r="26" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="27" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="21" t="s">
+      <c r="B27" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="C27" s="22"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="22"/>
-      <c r="F27" s="22"/>
-      <c r="G27" s="22"/>
-      <c r="H27" s="22"/>
-      <c r="I27" s="22"/>
-      <c r="J27" s="22"/>
-      <c r="K27" s="22"/>
-      <c r="L27" s="22"/>
-      <c r="M27" s="22"/>
-      <c r="N27" s="23"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="28"/>
+      <c r="H27" s="28"/>
+      <c r="I27" s="28"/>
+      <c r="J27" s="28"/>
+      <c r="K27" s="28"/>
+      <c r="L27" s="28"/>
+      <c r="M27" s="28"/>
+      <c r="N27" s="29"/>
     </row>
     <row r="28" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="29" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C29" s="24" t="s">
+      <c r="C29" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="D29" s="25"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="24" t="s">
+      <c r="D29" s="31"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="G29" s="25"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="24" t="s">
+      <c r="G29" s="31"/>
+      <c r="H29" s="32"/>
+      <c r="I29" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="J29" s="25"/>
-      <c r="K29" s="26"/>
-      <c r="L29" s="24" t="s">
+      <c r="J29" s="31"/>
+      <c r="K29" s="32"/>
+      <c r="L29" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="M29" s="25"/>
-      <c r="N29" s="26"/>
+      <c r="M29" s="31"/>
+      <c r="N29" s="32"/>
     </row>
     <row r="30" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="1" t="s">
@@ -13453,83 +13452,83 @@
     </row>
     <row r="63" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="64" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B64" s="21" t="s">
+      <c r="B64" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="C64" s="22"/>
-      <c r="D64" s="22"/>
-      <c r="E64" s="22"/>
-      <c r="F64" s="22"/>
-      <c r="G64" s="22"/>
-      <c r="H64" s="22"/>
-      <c r="I64" s="22"/>
-      <c r="J64" s="22"/>
-      <c r="K64" s="22"/>
-      <c r="L64" s="22"/>
-      <c r="M64" s="22"/>
-      <c r="N64" s="23"/>
+      <c r="C64" s="28"/>
+      <c r="D64" s="28"/>
+      <c r="E64" s="28"/>
+      <c r="F64" s="28"/>
+      <c r="G64" s="28"/>
+      <c r="H64" s="28"/>
+      <c r="I64" s="28"/>
+      <c r="J64" s="28"/>
+      <c r="K64" s="28"/>
+      <c r="L64" s="28"/>
+      <c r="M64" s="28"/>
+      <c r="N64" s="29"/>
     </row>
     <row r="65" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="66" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C66" s="24" t="s">
+      <c r="C66" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="D66" s="25"/>
-      <c r="E66" s="26"/>
-      <c r="F66" s="24" t="s">
+      <c r="D66" s="31"/>
+      <c r="E66" s="32"/>
+      <c r="F66" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="G66" s="25"/>
-      <c r="H66" s="26"/>
-      <c r="I66" s="24" t="s">
+      <c r="G66" s="31"/>
+      <c r="H66" s="32"/>
+      <c r="I66" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="J66" s="25"/>
-      <c r="K66" s="26"/>
-      <c r="L66" s="24" t="s">
+      <c r="J66" s="31"/>
+      <c r="K66" s="32"/>
+      <c r="L66" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="M66" s="25"/>
-      <c r="N66" s="26"/>
+      <c r="M66" s="31"/>
+      <c r="N66" s="32"/>
     </row>
     <row r="67" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B67" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C67" s="30" t="s">
+      <c r="C67" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D67" s="31" t="s">
+      <c r="D67" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="E67" s="28" t="s">
+      <c r="E67" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="F67" s="32" t="s">
+      <c r="F67" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="G67" s="33" t="s">
+      <c r="G67" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="H67" s="29" t="s">
+      <c r="H67" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="I67" s="30" t="s">
+      <c r="I67" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="J67" s="31" t="s">
+      <c r="J67" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="K67" s="28" t="s">
+      <c r="K67" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="L67" s="33" t="s">
+      <c r="L67" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="M67" s="33" t="s">
+      <c r="M67" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="N67" s="29" t="s">
+      <c r="N67" s="22" t="s">
         <v>13</v>
       </c>
     </row>
@@ -13544,7 +13543,7 @@
         <v>190370.30832400001</v>
       </c>
       <c r="E68" s="19">
-        <f>C$68/C68</f>
+        <f t="shared" ref="E68:E77" si="8">C$68/C68</f>
         <v>1</v>
       </c>
       <c r="F68" s="17">
@@ -13554,7 +13553,7 @@
         <v>167420.337218</v>
       </c>
       <c r="H68" s="19">
-        <f>F$68/F68</f>
+        <f t="shared" ref="H68:H77" si="9">F$68/F68</f>
         <v>1</v>
       </c>
       <c r="I68" s="17">
@@ -13564,19 +13563,19 @@
         <v>159403.70262900001</v>
       </c>
       <c r="K68" s="19">
-        <f>I$68/I68</f>
+        <f t="shared" ref="K68:K76" si="10">I$68/I68</f>
         <v>1</v>
       </c>
       <c r="L68" s="17">
-        <f t="shared" ref="L68:L77" si="8">AVERAGE(C68,F68,I68)</f>
+        <f t="shared" ref="L68:L77" si="11">AVERAGE(C68,F68,I68)</f>
         <v>583.30899999999997</v>
       </c>
       <c r="M68" s="18">
-        <f t="shared" ref="M68:M77" si="9">AVERAGE(D68,G68,J68)</f>
+        <f t="shared" ref="M68:M77" si="12">AVERAGE(D68,G68,J68)</f>
         <v>172398.11605700001</v>
       </c>
       <c r="N68" s="19">
-        <f>L$68/L68</f>
+        <f t="shared" ref="N68:N77" si="13">L$68/L68</f>
         <v>1</v>
       </c>
     </row>
@@ -13587,43 +13586,43 @@
       <c r="C69" s="9">
         <v>397.154</v>
       </c>
-      <c r="D69" s="27">
+      <c r="D69" s="10">
         <v>251791.49649799999</v>
       </c>
       <c r="E69" s="11">
-        <f>C$68/C69</f>
+        <f t="shared" si="8"/>
         <v>1.3226380698671045</v>
       </c>
       <c r="F69" s="9">
         <v>447.46</v>
       </c>
-      <c r="G69" s="27">
+      <c r="G69" s="10">
         <v>223483.663344</v>
       </c>
       <c r="H69" s="11">
-        <f>F$68/F69</f>
+        <f t="shared" si="9"/>
         <v>1.3348634514816968</v>
       </c>
       <c r="I69" s="9">
         <v>449.56099999999998</v>
       </c>
-      <c r="J69" s="27">
+      <c r="J69" s="10">
         <v>222439.22404299999</v>
       </c>
       <c r="K69" s="11">
-        <f>I$68/I69</f>
+        <f t="shared" si="10"/>
         <v>1.3954457793269435</v>
       </c>
       <c r="L69" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>431.39166666666665</v>
       </c>
-      <c r="M69" s="27">
-        <f t="shared" si="9"/>
+      <c r="M69" s="10">
+        <f t="shared" si="12"/>
         <v>232571.46129500002</v>
       </c>
       <c r="N69" s="11">
-        <f>L$68/L69</f>
+        <f t="shared" si="13"/>
         <v>1.3521563930689435</v>
       </c>
     </row>
@@ -13634,43 +13633,43 @@
       <c r="C70" s="9">
         <v>205.49</v>
       </c>
-      <c r="D70" s="27">
+      <c r="D70" s="10">
         <v>486641.685727</v>
       </c>
       <c r="E70" s="11">
-        <f>C$68/C70</f>
+        <f t="shared" si="8"/>
         <v>2.5562849773711616</v>
       </c>
       <c r="F70" s="9">
         <v>238.86600000000001</v>
       </c>
-      <c r="G70" s="27">
+      <c r="G70" s="10">
         <v>418644.76317300001</v>
       </c>
       <c r="H70" s="11">
-        <f>F$68/F70</f>
+        <f t="shared" si="9"/>
         <v>2.5005567975350194</v>
       </c>
       <c r="I70" s="9">
         <v>239.64</v>
       </c>
-      <c r="J70" s="27">
+      <c r="J70" s="10">
         <v>417292.60557499999</v>
       </c>
       <c r="K70" s="11">
-        <f>I$68/I70</f>
+        <f t="shared" si="10"/>
         <v>2.6178350859622768</v>
       </c>
       <c r="L70" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>227.99866666666665</v>
       </c>
-      <c r="M70" s="27">
-        <f t="shared" si="9"/>
+      <c r="M70" s="10">
+        <f t="shared" si="12"/>
         <v>440859.68482499995</v>
       </c>
       <c r="N70" s="11">
-        <f>L$68/L70</f>
+        <f t="shared" si="13"/>
         <v>2.5583877683495224</v>
       </c>
     </row>
@@ -13681,43 +13680,43 @@
       <c r="C71" s="9">
         <v>138.69200000000001</v>
       </c>
-      <c r="D71" s="27">
+      <c r="D71" s="10">
         <v>721016.92226699996</v>
       </c>
       <c r="E71" s="11">
-        <f>C$68/C71</f>
+        <f t="shared" si="8"/>
         <v>3.7874643094050127</v>
       </c>
       <c r="F71" s="9">
         <v>147.624</v>
       </c>
-      <c r="G71" s="27">
+      <c r="G71" s="10">
         <v>677396.62927399995</v>
       </c>
       <c r="H71" s="11">
-        <f>F$68/F71</f>
+        <f t="shared" si="9"/>
         <v>4.0460765187232433</v>
       </c>
       <c r="I71" s="9">
         <v>153.61000000000001</v>
       </c>
-      <c r="J71" s="27">
+      <c r="J71" s="10">
         <v>650999.28390100005</v>
       </c>
       <c r="K71" s="11">
-        <f>I$68/I71</f>
+        <f t="shared" si="10"/>
         <v>4.0839658876375227</v>
       </c>
       <c r="L71" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>146.64200000000002</v>
       </c>
-      <c r="M71" s="27">
-        <f t="shared" si="9"/>
+      <c r="M71" s="10">
+        <f t="shared" si="12"/>
         <v>683137.61181400006</v>
       </c>
       <c r="N71" s="11">
-        <f>L$68/L71</f>
+        <f t="shared" si="13"/>
         <v>3.9777758077494845</v>
       </c>
     </row>
@@ -13728,43 +13727,43 @@
       <c r="C72" s="9">
         <v>66.287000000000006</v>
       </c>
-      <c r="D72" s="27">
+      <c r="D72" s="10">
         <v>1508591.4281840001</v>
       </c>
       <c r="E72" s="11">
-        <f>C$68/C72</f>
+        <f t="shared" si="8"/>
         <v>7.9244949990194158</v>
       </c>
       <c r="F72" s="9">
         <v>88.302999999999997</v>
       </c>
-      <c r="G72" s="27">
+      <c r="G72" s="10">
         <v>1132464.3556840001</v>
       </c>
       <c r="H72" s="11">
-        <f>F$68/F72</f>
+        <f t="shared" si="9"/>
         <v>6.7641869472158369</v>
       </c>
       <c r="I72" s="9">
         <v>95.686000000000007</v>
       </c>
-      <c r="J72" s="27">
+      <c r="J72" s="10">
         <v>1045084.965408</v>
       </c>
       <c r="K72" s="11">
-        <f>I$68/I72</f>
+        <f t="shared" si="10"/>
         <v>6.5562151202892789</v>
       </c>
       <c r="L72" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>83.425333333333342</v>
       </c>
-      <c r="M72" s="27">
-        <f t="shared" si="9"/>
+      <c r="M72" s="10">
+        <f t="shared" si="12"/>
         <v>1228713.5830920001</v>
       </c>
       <c r="N72" s="11">
-        <f>L$68/L72</f>
+        <f t="shared" si="13"/>
         <v>6.9919888443158742</v>
       </c>
     </row>
@@ -13775,43 +13774,43 @@
       <c r="C73" s="9">
         <v>46.829000000000001</v>
       </c>
-      <c r="D73" s="27">
+      <c r="D73" s="10">
         <v>2135428.900895</v>
       </c>
       <c r="E73" s="11">
-        <f>C$68/C73</f>
+        <f t="shared" si="8"/>
         <v>11.217215827799015</v>
       </c>
       <c r="F73" s="9">
         <v>67.709000000000003</v>
       </c>
-      <c r="G73" s="27">
+      <c r="G73" s="10">
         <v>1476908.5350540001</v>
       </c>
       <c r="H73" s="11">
-        <f>F$68/F73</f>
+        <f t="shared" si="9"/>
         <v>8.8215451417093735</v>
       </c>
       <c r="I73" s="9">
         <v>69.363</v>
       </c>
-      <c r="J73" s="27">
+      <c r="J73" s="10">
         <v>1441690.8149880001</v>
       </c>
       <c r="K73" s="11">
-        <f>I$68/I73</f>
+        <f t="shared" si="10"/>
         <v>9.044274324928276</v>
       </c>
       <c r="L73" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>61.300333333333334</v>
       </c>
-      <c r="M73" s="27">
-        <f t="shared" si="9"/>
+      <c r="M73" s="10">
+        <f t="shared" si="12"/>
         <v>1684676.0836456667</v>
       </c>
       <c r="N73" s="11">
-        <f>L$68/L73</f>
+        <f t="shared" si="13"/>
         <v>9.5155926286425849</v>
       </c>
     </row>
@@ -13822,43 +13821,43 @@
       <c r="C74" s="9">
         <v>55.463999999999999</v>
       </c>
-      <c r="D74" s="27">
+      <c r="D74" s="10">
         <v>1802971.296697</v>
       </c>
       <c r="E74" s="11">
-        <f>C$68/C74</f>
+        <f t="shared" si="8"/>
         <v>9.470845954132411</v>
       </c>
       <c r="F74" s="9">
         <v>76.522000000000006</v>
       </c>
-      <c r="G74" s="27">
+      <c r="G74" s="10">
         <v>1306796.649373</v>
       </c>
       <c r="H74" s="11">
-        <f>F$68/F74</f>
+        <f t="shared" si="9"/>
         <v>7.8055722537309524</v>
       </c>
       <c r="I74" s="9">
         <v>79.194000000000003</v>
       </c>
-      <c r="J74" s="27">
+      <c r="J74" s="10">
         <v>1262721.923378</v>
       </c>
       <c r="K74" s="11">
-        <f>I$68/I74</f>
+        <f t="shared" si="10"/>
         <v>7.921534459681288</v>
       </c>
       <c r="L74" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>70.393333333333331</v>
       </c>
-      <c r="M74" s="27">
-        <f t="shared" si="9"/>
+      <c r="M74" s="10">
+        <f t="shared" si="12"/>
         <v>1457496.6231493335</v>
       </c>
       <c r="N74" s="11">
-        <f>L$68/L74</f>
+        <f t="shared" si="13"/>
         <v>8.2864239037787666</v>
       </c>
     </row>
@@ -13869,43 +13868,43 @@
       <c r="C75" s="9">
         <v>46.893000000000001</v>
       </c>
-      <c r="D75" s="27">
+      <c r="D75" s="10">
         <v>2132514.4477849999</v>
       </c>
       <c r="E75" s="11">
-        <f>C$68/C75</f>
+        <f t="shared" si="8"/>
         <v>11.201906467916322</v>
       </c>
       <c r="F75" s="9">
         <v>65.373000000000005</v>
       </c>
-      <c r="G75" s="27">
+      <c r="G75" s="10">
         <v>1529660.109524</v>
       </c>
       <c r="H75" s="11">
-        <f>F$68/F75</f>
+        <f t="shared" si="9"/>
         <v>9.1367690024933843</v>
       </c>
       <c r="I75" s="9">
         <v>63.960999999999999</v>
       </c>
-      <c r="J75" s="27">
+      <c r="J75" s="10">
         <v>1563452.7290070001</v>
       </c>
       <c r="K75" s="11">
-        <f>I$68/I75</f>
+        <f t="shared" si="10"/>
         <v>9.8081330810962921</v>
       </c>
       <c r="L75" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>58.742333333333335</v>
       </c>
-      <c r="M75" s="27">
-        <f t="shared" si="9"/>
+      <c r="M75" s="10">
+        <f t="shared" si="12"/>
         <v>1741875.7621053334</v>
       </c>
       <c r="N75" s="11">
-        <f>L$68/L75</f>
+        <f t="shared" si="13"/>
         <v>9.9299596543094975</v>
       </c>
     </row>
@@ -13916,43 +13915,43 @@
       <c r="C76" s="9">
         <v>41.402999999999999</v>
       </c>
-      <c r="D76" s="27">
+      <c r="D76" s="10">
         <v>2415283.9166239998</v>
       </c>
       <c r="E76" s="11">
-        <f>C$68/C76</f>
+        <f t="shared" si="8"/>
         <v>12.687269038475474</v>
       </c>
       <c r="F76" s="9">
         <v>66.623000000000005</v>
       </c>
-      <c r="G76" s="27">
+      <c r="G76" s="10">
         <v>1500960.614793</v>
       </c>
       <c r="H76" s="11">
-        <f>F$68/F76</f>
+        <f t="shared" si="9"/>
         <v>8.9653422992059788</v>
       </c>
       <c r="I76" s="9">
         <v>67.301000000000002</v>
       </c>
-      <c r="J76" s="27">
+      <c r="J76" s="10">
         <v>1485862.0228530001</v>
       </c>
       <c r="K76" s="11">
-        <f>I$68/I76</f>
+        <f t="shared" si="10"/>
         <v>9.3213770969227792</v>
       </c>
       <c r="L76" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>58.44233333333333</v>
       </c>
-      <c r="M76" s="27">
-        <f t="shared" si="9"/>
+      <c r="M76" s="10">
+        <f t="shared" si="12"/>
         <v>1800702.1847566667</v>
       </c>
       <c r="N76" s="11">
-        <f>L$68/L76</f>
+        <f t="shared" si="13"/>
         <v>9.980932771335846</v>
       </c>
     </row>
@@ -13967,7 +13966,7 @@
         <v>2638104.7855219999</v>
       </c>
       <c r="E77" s="16">
-        <f>C$68/C77</f>
+        <f t="shared" si="8"/>
         <v>13.858092599920855</v>
       </c>
       <c r="F77" s="14">
@@ -13977,37 +13976,37 @@
         <v>1448037.1855949999</v>
       </c>
       <c r="H77" s="16">
-        <f>F$68/F77</f>
+        <f t="shared" si="9"/>
         <v>8.586802760207016</v>
       </c>
       <c r="I77" s="14"/>
       <c r="J77" s="15"/>
       <c r="K77" s="16"/>
       <c r="L77" s="14">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>53.732500000000002</v>
       </c>
       <c r="M77" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>2043070.9855585</v>
       </c>
       <c r="N77" s="16">
-        <f>L$68/L77</f>
+        <f t="shared" si="13"/>
         <v>10.855794909970687</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B27:N27"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="F29:H29"/>
+    <mergeCell ref="I29:K29"/>
+    <mergeCell ref="L29:N29"/>
     <mergeCell ref="B64:N64"/>
     <mergeCell ref="C66:E66"/>
     <mergeCell ref="F66:H66"/>
     <mergeCell ref="I66:K66"/>
     <mergeCell ref="L66:N66"/>
-    <mergeCell ref="B27:N27"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="F29:H29"/>
-    <mergeCell ref="I29:K29"/>
-    <mergeCell ref="L29:N29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>